<commit_message>
[Modified]: Chỉnh sửa Achievement
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/Achievement/Achievement.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/Achievement/Achievement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\To-Do-App\ToDoApp-Doc\Document\Diagram\Thiết Kế Phần Mềm\Thiết Kế Xử Lý\Achievement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{042641D1-616F-44B0-92D4-304EF00A110C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE90D3FE-6E60-4D66-A9C7-1C4ED04F8E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="151">
   <si>
     <t>DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -469,6 +469,31 @@
   <si>
     <t>AC00001</t>
   </si>
+  <si>
+    <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU DOUBLE</t>
+  </si>
+  <si>
+    <t>Tỉ lệ Achievement
+đã hoàn thành so
+với tổng Achievement</t>
+  </si>
+  <si>
+    <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU BOOLEAN</t>
+  </si>
+  <si>
+    <t>achievementStatus</t>
+  </si>
+  <si>
+    <t>0 : Chưa hoàn thành
+1 : Đã hoàn thành</t>
+  </si>
+  <si>
+    <t>shareStatus</t>
+  </si>
+  <si>
+    <t>0 :Chưa share
+1 : Đã share</t>
+  </si>
 </sst>
 </file>
 
@@ -779,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -937,10 +962,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -952,11 +995,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -979,29 +1028,11 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1283,8 +1314,8 @@
   </sheetPr>
   <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1317,48 +1348,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="45" customHeight="1">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
       <c r="E1" s="9"/>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
       <c r="R1" s="4"/>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="54" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
       <c r="Y1" s="4"/>
-      <c r="Z1" s="53" t="s">
+      <c r="Z1" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="74"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="74"/>
-      <c r="AF1" s="53"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="55"/>
+      <c r="AF1" s="54"/>
     </row>
     <row r="2" spans="1:32" ht="26.25" customHeight="1">
       <c r="A2" s="47" t="s">
@@ -1451,16 +1482,16 @@
       </c>
     </row>
     <row r="3" spans="1:32" ht="77.099999999999994" customHeight="1">
-      <c r="A3" s="56">
+      <c r="A3" s="62">
         <v>1</v>
       </c>
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="D3" s="67"/>
+      <c r="D3" s="58"/>
       <c r="E3" s="10"/>
       <c r="F3" s="23">
         <v>1</v>
@@ -1533,10 +1564,10 @@
       <c r="AF3" s="34"/>
     </row>
     <row r="4" spans="1:32" ht="56.4" customHeight="1">
-      <c r="A4" s="70"/>
-      <c r="B4" s="72"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="68"/>
+      <c r="A4" s="64"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="59"/>
       <c r="E4" s="9"/>
       <c r="F4" s="13">
         <v>2</v>
@@ -1553,19 +1584,19 @@
       </c>
       <c r="K4" s="25"/>
       <c r="L4" s="4"/>
-      <c r="M4" s="56">
+      <c r="M4" s="62">
         <v>2</v>
       </c>
-      <c r="N4" s="56" t="s">
+      <c r="N4" s="62" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="56" t="s">
+      <c r="O4" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="P4" s="58" t="s">
+      <c r="P4" s="56" t="s">
         <v>131</v>
       </c>
-      <c r="Q4" s="56"/>
+      <c r="Q4" s="62"/>
       <c r="R4" s="4"/>
       <c r="S4" s="23">
         <v>2</v>
@@ -1605,10 +1636,10 @@
       <c r="AF4" s="25"/>
     </row>
     <row r="5" spans="1:32" ht="51.6" customHeight="1">
-      <c r="A5" s="57"/>
-      <c r="B5" s="73"/>
-      <c r="C5" s="62"/>
-      <c r="D5" s="69"/>
+      <c r="A5" s="63"/>
+      <c r="B5" s="67"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="9"/>
       <c r="F5" s="23">
         <v>3</v>
@@ -1625,11 +1656,11 @@
       </c>
       <c r="K5" s="23"/>
       <c r="L5" s="4"/>
-      <c r="M5" s="57"/>
-      <c r="N5" s="57"/>
-      <c r="O5" s="57"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="57"/>
+      <c r="M5" s="63"/>
+      <c r="N5" s="63"/>
+      <c r="O5" s="63"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="63"/>
       <c r="R5" s="4"/>
       <c r="S5" s="23">
         <v>3</v>
@@ -1744,14 +1775,14 @@
       </c>
       <c r="D7" s="16"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="66" t="s">
+      <c r="F7" s="74" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
       <c r="L7" s="4"/>
       <c r="M7" s="16">
         <v>4</v>
@@ -1887,16 +1918,16 @@
       <c r="AF8" s="36"/>
     </row>
     <row r="9" spans="1:32" ht="48.9" customHeight="1">
-      <c r="A9" s="56">
+      <c r="A9" s="62">
         <v>5</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="B9" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="55"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="9"/>
       <c r="F9" s="13">
         <v>1</v>
@@ -1957,10 +1988,10 @@
       <c r="AF9" s="36"/>
     </row>
     <row r="10" spans="1:32" ht="58.2" customHeight="1">
-      <c r="A10" s="70"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="55"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="61"/>
       <c r="E10" s="9"/>
       <c r="F10" s="13">
         <v>2</v>
@@ -2019,10 +2050,10 @@
       <c r="AF10" s="36"/>
     </row>
     <row r="11" spans="1:32" ht="43.8" customHeight="1">
-      <c r="A11" s="57"/>
-      <c r="B11" s="57"/>
-      <c r="C11" s="65"/>
-      <c r="D11" s="55"/>
+      <c r="A11" s="63"/>
+      <c r="B11" s="63"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="61"/>
       <c r="E11" s="9"/>
       <c r="F11" s="13">
         <v>3</v>
@@ -2148,14 +2179,14 @@
       <c r="C13" s="21"/>
       <c r="D13" s="16"/>
       <c r="E13" s="9"/>
-      <c r="F13" s="53" t="s">
+      <c r="F13" s="54" t="s">
         <v>106</v>
       </c>
-      <c r="G13" s="54"/>
-      <c r="H13" s="54"/>
-      <c r="I13" s="54"/>
-      <c r="J13" s="54"/>
-      <c r="K13" s="54"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
       <c r="L13" s="4"/>
       <c r="M13" s="20">
         <v>10</v>
@@ -2271,16 +2302,16 @@
       <c r="AF14" s="36"/>
     </row>
     <row r="15" spans="1:32" ht="45.6" customHeight="1">
-      <c r="A15" s="56">
+      <c r="A15" s="62">
         <v>9</v>
       </c>
-      <c r="B15" s="56" t="s">
+      <c r="B15" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="C15" s="58" t="s">
+      <c r="C15" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="56"/>
+      <c r="D15" s="62"/>
       <c r="E15" s="9"/>
       <c r="F15" s="8">
         <v>1</v>
@@ -2339,10 +2370,10 @@
       <c r="AF15" s="36"/>
     </row>
     <row r="16" spans="1:32" ht="32.1" customHeight="1">
-      <c r="A16" s="57"/>
-      <c r="B16" s="57"/>
-      <c r="C16" s="59"/>
-      <c r="D16" s="57"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="63"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="9"/>
       <c r="F16" s="8">
         <v>2</v>
@@ -2436,14 +2467,14 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="53" t="s">
+      <c r="F18" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
       <c r="L18" s="4"/>
       <c r="M18" s="37">
         <v>15</v>
@@ -2607,7 +2638,14 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="42"/>
+      <c r="F22" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="61"/>
+      <c r="K22" s="61"/>
       <c r="L22" s="4"/>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
@@ -2636,7 +2674,24 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="42"/>
+      <c r="F23" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I23" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="L23" s="4"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
@@ -2659,13 +2714,28 @@
       <c r="AE23" s="7"/>
       <c r="AF23" s="6"/>
     </row>
-    <row r="24" spans="1:32" ht="27" customHeight="1">
+    <row r="24" spans="1:32" ht="54.6" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
-      <c r="F24" s="43"/>
+      <c r="F24" s="25">
+        <v>1</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>79</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="I24" s="26"/>
+      <c r="J24" s="25">
+        <v>0</v>
+      </c>
+      <c r="K24" s="26" t="s">
+        <v>145</v>
+      </c>
       <c r="L24" s="4"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
@@ -2723,12 +2793,14 @@
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
+      <c r="F26" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="G26" s="76"/>
+      <c r="H26" s="76"/>
+      <c r="I26" s="76"/>
+      <c r="J26" s="76"/>
+      <c r="K26" s="76"/>
       <c r="L26" s="4"/>
       <c r="M26" s="2"/>
       <c r="N26" s="2"/>
@@ -2757,12 +2829,24 @@
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="12"/>
-      <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
+      <c r="F27" s="27" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>7</v>
+      </c>
       <c r="L27" s="4"/>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
@@ -2785,18 +2869,28 @@
       <c r="AE27" s="7"/>
       <c r="AF27" s="6"/>
     </row>
-    <row r="28" spans="1:32" ht="27" customHeight="1">
+    <row r="28" spans="1:32" ht="53.4" customHeight="1">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-      <c r="I28" s="12"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="F28" s="25">
+        <v>1</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>147</v>
+      </c>
+      <c r="H28" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I28" s="26"/>
+      <c r="J28" s="25">
+        <v>0</v>
+      </c>
+      <c r="K28" s="26" t="s">
+        <v>148</v>
+      </c>
       <c r="L28" s="4"/>
       <c r="M28" s="2"/>
       <c r="N28" s="2"/>
@@ -2813,18 +2907,28 @@
       <c r="Y28" s="4"/>
       <c r="Z28" s="4"/>
     </row>
-    <row r="29" spans="1:32" ht="27" customHeight="1">
+    <row r="29" spans="1:32" ht="32.4" customHeight="1">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="12"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="F29" s="53">
+        <v>2</v>
+      </c>
+      <c r="G29" s="53" t="s">
+        <v>149</v>
+      </c>
+      <c r="H29" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="24"/>
+      <c r="J29" s="53">
+        <v>0</v>
+      </c>
+      <c r="K29" s="24" t="s">
+        <v>150</v>
+      </c>
       <c r="L29" s="4"/>
       <c r="M29" s="2"/>
       <c r="N29" s="2"/>
@@ -30142,12 +30246,19 @@
       <c r="Z1004" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:K1"/>
-    <mergeCell ref="M1:Q1"/>
-    <mergeCell ref="S1:X1"/>
-    <mergeCell ref="Z1:AF1"/>
+  <mergeCells count="27">
+    <mergeCell ref="F22:K22"/>
+    <mergeCell ref="F26:K26"/>
+    <mergeCell ref="F13:K13"/>
+    <mergeCell ref="F18:K18"/>
+    <mergeCell ref="M4:M5"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="P4:P5"/>
+    <mergeCell ref="Q4:Q5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="F7:K7"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D3:D5"/>
     <mergeCell ref="D9:D11"/>
@@ -30158,16 +30269,11 @@
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="B15:B16"/>
-    <mergeCell ref="P4:P5"/>
-    <mergeCell ref="Q4:Q5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="F7:K7"/>
-    <mergeCell ref="F13:K13"/>
-    <mergeCell ref="F18:K18"/>
-    <mergeCell ref="M4:M5"/>
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:O5"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="S1:X1"/>
+    <mergeCell ref="Z1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>